<commit_message>
Proceso de SBS_back a una clase y a un objeto
</commit_message>
<xml_diff>
--- a/precios.xlsx
+++ b/precios.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K58"/>
+  <dimension ref="A1:K64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,40 +496,40 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45020</v>
+        <v>45021</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>DFB Pokal</t>
+          <t>Copa del Rey</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Barcelona</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>SC Freiburg</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>1-2</t>
+          <t>0-4</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>213.2</v>
+        <v>29.59</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -549,52 +549,54 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>SC Freiburg</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Villarreal</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>2-3</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>216.4</v>
+        <v>29.37</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Perdido</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr"/>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>-0.7434944237918177</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45027</v>
+        <v>45028</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -603,22 +605,22 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Manchester City</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Chelsea</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>3-0</t>
+          <t>2-0</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -627,21 +629,19 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>216.4</v>
+        <v>29.92</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="K4" t="n">
-        <v>1.500938086303948</v>
-      </c>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -649,52 +649,52 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Cádiz</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Hoffenheim</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1-1</t>
+          <t>0-2</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>216.5</v>
+        <v>30.85</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Empatado</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45035</v>
+        <v>45034</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -703,40 +703,40 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Chelsea</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Manchester City</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1-1</t>
+          <t>0-2</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>221.75</v>
+        <v>31.08</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Empatado</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K6" t="inlineStr"/>
@@ -747,85 +747,85 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Mainz 05</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Celta</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>3-1</t>
+          <t>2-0</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>223.75</v>
+        <v>31.82</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45046</v>
+        <v>45041</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Girona</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Hertha BSC</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2-0</t>
+          <t>4-2</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="H8" t="n">
-        <v>222.35</v>
+        <v>31.37</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -834,38 +834,40 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
-        </is>
-      </c>
-      <c r="K8" t="inlineStr"/>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="K8" t="n">
+        <v>6.050703079658669</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45052</v>
+        <v>45045</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Almería</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1-2</t>
+          <t>4-2</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -874,7 +876,7 @@
         </is>
       </c>
       <c r="H9" t="n">
-        <v>217</v>
+        <v>31.06</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -890,31 +892,31 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45059</v>
+        <v>45048</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Real Sociedad</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Schalke 04</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>6-0</t>
+          <t>2-0</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -923,7 +925,7 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>210.55</v>
+        <v>31.06</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -936,45 +938,45 @@
         </is>
       </c>
       <c r="K10" t="n">
-        <v>-2.972350230414742</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45066</v>
+        <v>45052</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Copa del Rey</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>RB Leipzig</t>
+          <t>Osasuna</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1-3</t>
+          <t>2-1</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>211.6</v>
+        <v>31.97</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -990,26 +992,26 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45073</v>
+        <v>45055</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Champions League</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Köln</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Manchester City</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1-2</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1019,60 +1021,60 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>207.75</v>
+        <v>31.99</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Empatado</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45125</v>
+        <v>45059</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Partidos Amistosos</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>FC Rottach-Egern</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Getafe</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0-27</t>
+          <t>1-0</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>27</t>
-        </is>
-      </c>
       <c r="H13" t="n">
-        <v>210.8</v>
+        <v>30.76</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
@@ -1088,138 +1090,140 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45133</v>
+        <v>45063</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Partidos Amistosos</t>
+          <t>Champions League</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Manchester City</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Manchester City</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1-2</t>
+          <t>4-0</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>215.8</v>
+        <v>30.99</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Perdido</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr"/>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="K14" t="n">
+        <v>-2.317649470631004</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45136</v>
+        <v>45067</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Partidos Amistosos</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Kawasaki Frontale</t>
+          <t>Valencia</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>1-0</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="H15" t="n">
-        <v>217.4</v>
+        <v>31.49</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Perdido</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45140</v>
+        <v>45070</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Partidos Amistosos</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Rayo Vallecano</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>2-1</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H16" t="n">
-        <v>211.75</v>
+        <v>30.82</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
@@ -1235,31 +1239,31 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45145</v>
+        <v>45073</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Partidos Amistosos</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Sevilla</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Monaco</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>4-2</t>
+          <t>1-2</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1268,107 +1272,105 @@
         </is>
       </c>
       <c r="H17" t="n">
-        <v>215.05</v>
+        <v>31.18</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="K17" t="n">
-        <v>7.29034333783178</v>
-      </c>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45150</v>
+        <v>45081</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Supercopa de Alemania</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>RB Leipzig</t>
+          <t>Athletic</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0-3</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H18" t="n">
-        <v>224.3</v>
+        <v>31.4</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Empatado</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45156</v>
+        <v>45131</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Soccer Champions Tour</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Milan</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0-4</t>
+          <t>3-2</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H19" t="n">
-        <v>221.15</v>
+        <v>30.45</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
@@ -1384,40 +1386,40 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45157</v>
+        <v>45134</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Partidos Amistosos</t>
+          <t>Soccer Champions Tour</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Weinbeisser Kaltern</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Manchester United</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>1-6</t>
+          <t>2-0</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H20" t="n">
-        <v>220.8</v>
+        <v>31.84</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
@@ -1433,26 +1435,26 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45165</v>
+        <v>45136</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Soccer Champions Tour</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Barcelona</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>FC Augsburg</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>3-1</t>
+          <t>3-0</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1462,11 +1464,11 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H21" t="n">
-        <v>224.7</v>
+        <v>31.79</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
@@ -1479,134 +1481,134 @@
         </is>
       </c>
       <c r="K21" t="n">
-        <v>3.549882246720995</v>
+        <v>9.347310878457476</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45171</v>
+        <v>45141</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Soccer Champions Tour</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>B. Mönchengladbach</t>
+          <t>Juventus</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1-2</t>
+          <t>3-1</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H22" t="n">
-        <v>223.3</v>
+        <v>31.15</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Perdido</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45184</v>
+        <v>45150</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Athletic</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>B. Leverkusen</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2-2</t>
+          <t>0-2</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
       <c r="H23" t="n">
-        <v>233.45</v>
+        <v>31.68</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Empatado</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45189</v>
+        <v>45157</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Champions League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Almería</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Manchester United</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>4-3</t>
+          <t>1-3</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1615,107 +1617,105 @@
         </is>
       </c>
       <c r="H24" t="n">
-        <v>231.4</v>
+        <v>31.31</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="K24" t="n">
-        <v>3.627407075682935</v>
-      </c>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45192</v>
+        <v>45163</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Celta</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>VfL Bochum</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>7-0</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H25" t="n">
-        <v>229.35</v>
+        <v>31.67</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45195</v>
+        <v>45171</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>DFB Pokal</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Preußen Münster</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Getafe</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>0-4</t>
+          <t>2-1</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H26" t="n">
-        <v>230.45</v>
+        <v>32.37</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
@@ -1731,26 +1731,26 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45199</v>
+        <v>45186</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>RB Leipzig</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Real Sociedad</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2-2</t>
+          <t>2-1</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1760,27 +1760,27 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H27" t="n">
-        <v>222.7</v>
+        <v>33.62</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Empatado</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45202</v>
+        <v>45189</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1789,17 +1789,17 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Kobenhavn</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Union Berlin</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1-2</t>
+          <t>1-0</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1809,11 +1809,11 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H28" t="n">
-        <v>220.95</v>
+        <v>34.36</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
@@ -1829,26 +1829,26 @@
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45207</v>
+        <v>45193</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Atlético</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>SC Freiburg</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>3-0</t>
+          <t>3-1</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -1858,11 +1858,11 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H29" t="n">
-        <v>222.5</v>
+        <v>33.83</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
@@ -1875,45 +1875,45 @@
         </is>
       </c>
       <c r="K29" t="n">
-        <v>-2.748256004724456</v>
+        <v>25.24798367063588</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45220</v>
+        <v>45196</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Mainz 05</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Las Palmas</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>1-3</t>
+          <t>2-0</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H30" t="n">
-        <v>217.8</v>
+        <v>33.8</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
@@ -1929,31 +1929,31 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45223</v>
+        <v>45199</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Champions League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Galatasaray SK</t>
+          <t>Girona</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1-3</t>
+          <t>0-3</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -1962,7 +1962,7 @@
         </is>
       </c>
       <c r="H31" t="n">
-        <v>218.15</v>
+        <v>33.72</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
@@ -1978,156 +1978,154 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>45227</v>
+        <v>45202</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Champions League</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Napoli</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Darmstadt 98</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>8-0</t>
+          <t>2-3</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H32" t="n">
-        <v>221.05</v>
+        <v>33.45</v>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="K32" t="n">
-        <v>2.821555205757071</v>
-      </c>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>45231</v>
+        <v>45206</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>DFB Pokal</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>1. FC Saarbrücken</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Osasuna</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>2-1</t>
+          <t>4-0</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H33" t="n">
-        <v>224.25</v>
+        <v>32.89</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>45234</v>
+        <v>45220</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>B. Dortmund</t>
+          <t>Sevilla</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>0-4</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H34" t="n">
-        <v>221.15</v>
+        <v>32.41</v>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Empatado</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>45238</v>
+        <v>45223</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -2136,73 +2134,71 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Sporting Braga</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Galatasaray SK</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>2-1</t>
+          <t>1-2</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="H35" t="n">
-        <v>220.75</v>
+        <v>32.62</v>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="K35" t="n">
-        <v>-0.1808727108297561</v>
-      </c>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>45241</v>
+        <v>45227</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Barcelona</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Heidenheim</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>4-2</t>
+          <t>1-2</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -2211,42 +2207,42 @@
         </is>
       </c>
       <c r="H36" t="n">
-        <v>221.4</v>
+        <v>33.74</v>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>45254</v>
+        <v>45235</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Köln</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Rayo Vallecano</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>0-0</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2256,27 +2252,27 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H37" t="n">
-        <v>232.7</v>
+        <v>33.5</v>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Empatado</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>45259</v>
+        <v>45238</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -2285,61 +2281,61 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Kobenhavn</t>
+          <t>Sporting Braga</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>0-0</t>
+          <t>3-0</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="H38" t="n">
-        <v>231</v>
+        <v>33.26</v>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>Empatado</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>45269</v>
+        <v>45241</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Eintracht Frankfurt</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Valencia</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -2358,44 +2354,42 @@
         </is>
       </c>
       <c r="H39" t="n">
-        <v>245.4</v>
+        <v>33.78</v>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="K39" t="n">
-        <v>5.45767082079932</v>
-      </c>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>45272</v>
+        <v>45256</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Champions League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Manchester United</t>
+          <t>Cádiz</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>0-3</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2405,11 +2399,11 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H40" t="n">
-        <v>245.5</v>
+        <v>36.41</v>
       </c>
       <c r="I40" t="inlineStr">
         <is>
@@ -2425,91 +2419,89 @@
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>45277</v>
+        <v>45259</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Champions League</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Stuttgart</t>
+          <t>Napoli</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>3-0</t>
+          <t>4-2</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H41" t="n">
-        <v>240.7</v>
+        <v>36.76</v>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="K41" t="n">
-        <v>-1.955193482688396</v>
-      </c>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>45280</v>
+        <v>45262</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Wolfsburg</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Granada</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>1-2</t>
+          <t>2-0</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H42" t="n">
-        <v>242.25</v>
+        <v>36.93</v>
       </c>
       <c r="I42" t="inlineStr">
         <is>
@@ -2518,28 +2510,28 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>45297</v>
+        <v>45269</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Partidos Amistosos</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Basel</t>
+          <t>Real Betis</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -2558,7 +2550,7 @@
         </is>
       </c>
       <c r="H43" t="n">
-        <v>244.55</v>
+        <v>37.46</v>
       </c>
       <c r="I43" t="inlineStr">
         <is>
@@ -2574,82 +2566,80 @@
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>45303</v>
+        <v>45272</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Champions League</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Union Berlin</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Hoffenheim</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>3-0</t>
+          <t>2-3</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="H44" t="n">
-        <v>241.7</v>
+        <v>37.98</v>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="K44" t="n">
-        <v>-0.2270381836945351</v>
-      </c>
+          <t>NO SE REALIZA OPERACION</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>45312</v>
+        <v>45277</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Villarreal</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>4-1</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
@@ -2658,7 +2648,7 @@
         </is>
       </c>
       <c r="H45" t="n">
-        <v>249.85</v>
+        <v>39.3</v>
       </c>
       <c r="I45" t="inlineStr">
         <is>
@@ -2667,98 +2657,96 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>45315</v>
+        <v>45281</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Deportivo Alavés</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Union Berlin</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>1-0</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H46" t="n">
-        <v>248.5</v>
+        <v>39.77</v>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="K46" t="n">
-        <v>-0.5403241945167078</v>
-      </c>
+          <t>NO SE REALIZA OPERACION</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>45318</v>
+        <v>45294</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>FC Augsburg</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Mallorca</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2-3</t>
+          <t>1-0</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H47" t="n">
-        <v>246.55</v>
+        <v>39.41</v>
       </c>
       <c r="I47" t="inlineStr">
         <is>
@@ -2767,102 +2755,100 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>45325</v>
+        <v>45297</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Copa del Rey</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Arandina</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>B. Mönchengladbach</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>3-1</t>
+          <t>1-3</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="H48" t="n">
-        <v>245.4</v>
+        <v>39.98</v>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="K48" t="n">
-        <v>-0.4664368282295704</v>
-      </c>
+          <t>NO SE REALIZA OPERACION</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>45332</v>
+        <v>45301</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Supercopa de España</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>B. Leverkusen</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Atlético</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>3-0</t>
+          <t>5-3</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="H49" t="n">
-        <v>246.25</v>
+        <v>38.977</v>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
@@ -2874,44 +2860,44 @@
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
-        <v>45336</v>
+        <v>45305</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Champions League</t>
+          <t>Supercopa de España</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Lazio</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Barcelona</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>1-0</t>
+          <t>4-1</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H50" t="n">
-        <v>244.6</v>
+        <v>39.797</v>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
@@ -2923,31 +2909,31 @@
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
-        <v>45340</v>
+        <v>45309</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Copa del Rey</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>VfL Bochum</t>
+          <t>Atlético</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>3-2</t>
+          <t>4-2</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -2956,7 +2942,7 @@
         </is>
       </c>
       <c r="H51" t="n">
-        <v>248.65</v>
+        <v>39.214</v>
       </c>
       <c r="I51" t="inlineStr">
         <is>
@@ -2965,185 +2951,187 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
-        </is>
-      </c>
-      <c r="K51" t="inlineStr"/>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="K51" t="n">
+        <v>153.5735694237965</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
-        <v>45346</v>
+        <v>45312</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>RB Leipzig</t>
+          <t>Almería</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>2-1</t>
+          <t>3-2</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="H52" t="n">
-        <v>245.65</v>
+        <v>39.75</v>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
-        <v>45352</v>
+        <v>45318</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>SC Freiburg</t>
+          <t>Las Palmas</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>2-2</t>
+          <t>1-2</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
       <c r="H53" t="n">
-        <v>251.8</v>
+        <v>35.66</v>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>Empatado</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
-        <v>45356</v>
+        <v>45323</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Champions League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Getafe</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Lazio</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>3-0</t>
+          <t>0-2</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H54" t="n">
-        <v>254.45</v>
+        <v>36.61</v>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
-        <v>45360</v>
+        <v>45326</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Mainz 05</t>
+          <t>Atlético</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>8-1</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
@@ -3152,11 +3140,11 @@
         </is>
       </c>
       <c r="H55" t="n">
-        <v>260.25</v>
+        <v>36.46</v>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Empatado</t>
         </is>
       </c>
       <c r="J55" t="inlineStr">
@@ -3168,40 +3156,40 @@
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
-        <v>45367</v>
+        <v>45332</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Darmstadt 98</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Girona</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>2-5</t>
+          <t>4-0</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H56" t="n">
-        <v>266.2</v>
+        <v>36.21</v>
       </c>
       <c r="I56" t="inlineStr">
         <is>
@@ -3217,26 +3205,26 @@
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
-        <v>45381</v>
+        <v>45335</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Champions League</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>RB Leipzig</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>B. Dortmund</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>0-2</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -3246,11 +3234,11 @@
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H57" t="n">
-        <v>273.9</v>
+        <v>36.39</v>
       </c>
       <c r="I57" t="inlineStr">
         <is>
@@ -3266,50 +3254,346 @@
     </row>
     <row r="58">
       <c r="A58" s="2" t="n">
-        <v>45388</v>
+        <v>45340</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Heidenheim</t>
+          <t>Rayo Vallecano</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>3-2</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H58" t="n">
+        <v>36.45</v>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>Empatado</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>NO SE REALIZA OPERACION</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="n">
+        <v>45347</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Primera División</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Sevilla</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>1-0</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H59" t="n">
+        <v>36.94</v>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>Ganado</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="n">
+        <v>45353</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Primera División</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>2-2</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="H58" t="inlineStr"/>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>Perdido</t>
-        </is>
-      </c>
-      <c r="J58" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="K58" t="inlineStr"/>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H60" t="n">
+        <v>37.74</v>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>Empatado</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>NO SE REALIZA OPERACION</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="n">
+        <v>45357</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Champions League</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>RB Leipzig</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>1-1</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H61" t="n">
+        <v>38.5</v>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>Empatado</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>NO SE REALIZA OPERACION</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="n">
+        <v>45361</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Primera División</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Celta</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>4-0</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H62" t="n">
+        <v>38.77</v>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>Ganado</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr"/>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="n">
+        <v>45367</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Primera División</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Osasuna</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>2-4</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H63" t="n">
+        <v>40.14</v>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>Ganado</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr"/>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="n">
+        <v>45382</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Primera División</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Athletic</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>2-0</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H64" t="n">
+        <v>38.48</v>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>Ganado</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Intefaz con vsualizacion de ticks y rentabilidad en el formulario solo de RSI para las estrategias normales y tambien hechos para las de futbol
</commit_message>
<xml_diff>
--- a/precios.xlsx
+++ b/precios.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K66"/>
+  <dimension ref="A1:K64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,26 +496,26 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45025</v>
+        <v>45024</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Arsenal</t>
+          <t>Villarreal</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2-2</t>
+          <t>2-3</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -525,15 +525,15 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>618.4</v>
+        <v>29.37</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Empatado</t>
+          <t>Perdido</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -545,40 +545,40 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>45033</v>
+        <v>45028</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Champions League</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Leeds United</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Chelsea</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1-6</t>
+          <t>2-0</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>642</v>
+        <v>29.92</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -594,31 +594,31 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>45038</v>
+        <v>45031</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Cádiz</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Nottingham Forest</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>3-2</t>
+          <t>0-2</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>632.4</v>
+        <v>30.85</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -643,31 +643,31 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>45042</v>
+        <v>45034</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Champions League</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>West Ham</t>
+          <t>Chelsea</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1-2</t>
+          <t>0-2</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -676,7 +676,7 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>634</v>
+        <v>31.08</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -692,40 +692,40 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>45046</v>
+        <v>45038</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Tottenham Hotspur</t>
+          <t>Celta</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>4-3</t>
+          <t>2-0</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>610.6</v>
+        <v>31.82</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -741,89 +741,91 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>45049</v>
+        <v>45041</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Girona</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Fulham</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1-0</t>
+          <t>4-2</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>611.4</v>
+        <v>31.37</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Perdido</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr"/>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="K7" t="n">
+        <v>6.050703079658669</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>45052</v>
+        <v>45045</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Brentford</t>
+          <t>Almería</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>1-0</t>
+          <t>4-2</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>604.6</v>
+        <v>31.06</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -839,80 +841,82 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>45061</v>
+        <v>45048</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Leicester</t>
+          <t>Real Sociedad</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0-3</t>
+          <t>2-0</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
       <c r="H9" t="n">
-        <v>619</v>
+        <v>31.06</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Perdido</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K9" t="inlineStr"/>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>45066</v>
+        <v>45052</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Copa del Rey</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Aston Villa</t>
+          <t>Osasuna</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1-1</t>
+          <t>2-1</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -921,56 +925,56 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>653.2</v>
+        <v>31.97</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Empatado</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>45074</v>
+        <v>45055</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Champions League</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Southampton</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Manchester City</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>4-4</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>643.2</v>
+        <v>31.99</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -986,40 +990,40 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>45126</v>
+        <v>45059</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Partidos Amistosos</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Karlsruher SC</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Getafe</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>2-4</t>
+          <t>1-0</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>706</v>
+        <v>30.76</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -1035,26 +1039,26 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>45131</v>
+        <v>45063</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Partidos Amistosos</t>
+          <t>Champions League</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Greuther Fürth</t>
+          <t>Manchester City</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>4-4</t>
+          <t>4-0</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1064,51 +1068,53 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>719.4</v>
+        <v>30.99</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Empatado</t>
+          <t>Perdido</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr"/>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="K13" t="n">
+        <v>-2.317649470631004</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>45137</v>
+        <v>45067</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Partidos Amistosos</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Valencia</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Leicester</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>4-0</t>
+          <t>1-0</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1117,107 +1123,105 @@
         </is>
       </c>
       <c r="H14" t="n">
-        <v>747.4</v>
+        <v>31.49</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Perdido</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>45140</v>
+        <v>45070</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Partidos Amistosos</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Bayern München</t>
+          <t>Rayo Vallecano</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>2-1</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H15" t="n">
-        <v>734.2</v>
+        <v>30.82</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="K15" t="n">
-        <v>128.8651630865327</v>
-      </c>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>45145</v>
+        <v>45073</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Partidos Amistosos</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Sevilla</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Darmstadt 98</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>3-1</t>
+          <t>1-2</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H16" t="n">
-        <v>747</v>
+        <v>31.18</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
@@ -1233,21 +1237,21 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>45151</v>
+        <v>45081</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Chelsea</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Athletic</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1266,7 +1270,7 @@
         </is>
       </c>
       <c r="H17" t="n">
-        <v>751.4</v>
+        <v>31.4</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
@@ -1282,26 +1286,26 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>45157</v>
+        <v>45131</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Soccer Champions Tour</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>AFC Bournemouth</t>
+          <t>Milan</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>3-1</t>
+          <t>3-2</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1311,11 +1315,11 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H18" t="n">
-        <v>719.4</v>
+        <v>30.45</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
@@ -1331,40 +1335,40 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>45165</v>
+        <v>45134</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Soccer Champions Tour</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Newcastle</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Manchester United</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1-2</t>
+          <t>2-0</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H19" t="n">
-        <v>723.8</v>
+        <v>31.84</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
@@ -1380,21 +1384,21 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>45172</v>
+        <v>45136</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Soccer Champions Tour</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Barcelona</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Aston Villa</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1413,105 +1417,107 @@
         </is>
       </c>
       <c r="H20" t="n">
-        <v>709.4</v>
+        <v>31.79</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Perdido</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K20" t="inlineStr"/>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="K20" t="n">
+        <v>9.347310878457476</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>45185</v>
+        <v>45141</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Soccer Champions Tour</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Wolves</t>
+          <t>Juventus</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1-3</t>
+          <t>3-1</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H21" t="n">
-        <v>737.2</v>
+        <v>31.15</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Perdido</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>45190</v>
+        <v>45150</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Europa League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>LASK</t>
+          <t>Athletic</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>1-3</t>
+          <t>0-2</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H22" t="n">
-        <v>753.4</v>
+        <v>31.68</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
@@ -1527,40 +1533,40 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>45193</v>
+        <v>45157</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Almería</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>West Ham</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>3-1</t>
+          <t>1-3</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="H23" t="n">
-        <v>749</v>
+        <v>31.31</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
@@ -1576,31 +1582,31 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>45196</v>
+        <v>45163</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>EFL Cup</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Celta</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Leicester</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>3-1</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1609,7 +1615,7 @@
         </is>
       </c>
       <c r="H24" t="n">
-        <v>750.2</v>
+        <v>31.67</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
@@ -1625,21 +1631,21 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>45199</v>
+        <v>45171</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Tottenham Hotspur</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Getafe</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1658,44 +1664,42 @@
         </is>
       </c>
       <c r="H25" t="n">
-        <v>753.8</v>
+        <v>32.37</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="K25" t="n">
-        <v>19.52125470182909</v>
-      </c>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>45204</v>
+        <v>45186</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Europa League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Union Saint-Gilloise</t>
+          <t>Real Sociedad</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>2-0</t>
+          <t>2-1</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -1705,11 +1709,11 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H26" t="n">
-        <v>749.4</v>
+        <v>33.62</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
@@ -1725,138 +1729,140 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>45207</v>
+        <v>45189</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Champions League</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Brighton &amp; Hove Albion</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Union Berlin</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2-2</t>
+          <t>1-0</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H27" t="n">
-        <v>738.2</v>
+        <v>34.36</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Empatado</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>45220</v>
+        <v>45193</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Atlético</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Everton</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2-0</t>
+          <t>3-1</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H28" t="n">
-        <v>717.4</v>
+        <v>33.83</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Perdido</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr"/>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="K28" t="n">
+        <v>25.24798367063588</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>45225</v>
+        <v>45196</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Europa League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Toulouse</t>
+          <t>Las Palmas</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>5-1</t>
+          <t>2-0</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H29" t="n">
-        <v>625.2</v>
+        <v>33.8</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
@@ -1872,40 +1878,40 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>45228</v>
+        <v>45199</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Girona</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Nottingham Forest</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>3-0</t>
+          <t>0-3</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
           <t>3</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="H30" t="n">
-        <v>620.4</v>
+        <v>33.72</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
@@ -1921,40 +1927,40 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>45231</v>
+        <v>45202</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>EFL Cup</t>
+          <t>Champions League</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>AFC Bournemouth</t>
+          <t>Napoli</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>1-2</t>
+          <t>2-3</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H31" t="n">
-        <v>611.6</v>
+        <v>33.45</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
@@ -1970,140 +1976,138 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>45235</v>
+        <v>45206</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Luton Town</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Osasuna</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>1-1</t>
+          <t>4-0</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H32" t="n">
-        <v>632</v>
+        <v>32.89</v>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>Empatado</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>45239</v>
+        <v>45220</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Europa League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Toulouse</t>
+          <t>Sevilla</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>3-2</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H33" t="n">
-        <v>627.2</v>
+        <v>32.41</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Empatado</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="K33" t="n">
-        <v>-24.91290795760242</v>
-      </c>
+          <t>NO SE REALIZA OPERACION</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>45242</v>
+        <v>45223</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Champions League</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Sporting Braga</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Brentford</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>3-0</t>
+          <t>1-2</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H34" t="n">
-        <v>628.4</v>
+        <v>32.62</v>
       </c>
       <c r="I34" t="inlineStr">
         <is>
@@ -2119,26 +2123,26 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>45255</v>
+        <v>45227</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Manchester City</t>
+          <t>Barcelona</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>1-1</t>
+          <t>1-2</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -2148,51 +2152,51 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H35" t="n">
-        <v>667.4</v>
+        <v>33.74</v>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>Empatado</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>NO SE REALIZA OPERACION</t>
+          <t>1</t>
         </is>
       </c>
       <c r="K35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>45260</v>
+        <v>45235</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Europa League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>LASK</t>
+          <t>Rayo Vallecano</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>4-0</t>
+          <t>0-0</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -2201,56 +2205,56 @@
         </is>
       </c>
       <c r="H36" t="n">
-        <v>653.2</v>
+        <v>33.5</v>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Empatado</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>45263</v>
+        <v>45238</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Champions League</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Fulham</t>
+          <t>Sporting Braga</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>4-3</t>
+          <t>3-0</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H37" t="n">
-        <v>653.2</v>
+        <v>33.26</v>
       </c>
       <c r="I37" t="inlineStr">
         <is>
@@ -2266,40 +2270,40 @@
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>45266</v>
+        <v>45241</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Sheffield United</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Valencia</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>0-2</t>
+          <t>5-1</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>5</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H38" t="n">
-        <v>663.4</v>
+        <v>33.78</v>
       </c>
       <c r="I38" t="inlineStr">
         <is>
@@ -2315,40 +2319,40 @@
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>45269</v>
+        <v>45256</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Crystal Palace</t>
+          <t>Cádiz</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>1-2</t>
+          <t>0-3</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H39" t="n">
-        <v>647</v>
+        <v>36.41</v>
       </c>
       <c r="I39" t="inlineStr">
         <is>
@@ -2364,95 +2368,93 @@
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>45274</v>
+        <v>45259</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Europa League</t>
+          <t>Champions League</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Union Saint-Gilloise</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Napoli</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>2-1</t>
+          <t>4-2</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
           <t>2</t>
         </is>
       </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="H40" t="n">
-        <v>655</v>
+        <v>36.76</v>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="K40" t="n">
-        <v>4.754377154869857</v>
-      </c>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>45277</v>
+        <v>45262</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Manchester United</t>
+          <t>Granada</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>0-0</t>
+          <t>2-0</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
       <c r="H41" t="n">
-        <v>645.8</v>
+        <v>36.93</v>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>Empatado</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
@@ -2464,31 +2466,31 @@
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>45280</v>
+        <v>45269</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>EFL Cup</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Betis</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>West Ham</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>5-1</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -2497,60 +2499,60 @@
         </is>
       </c>
       <c r="H42" t="n">
-        <v>661.8</v>
+        <v>37.46</v>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Empatado</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
-        <v>45283</v>
+        <v>45272</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Champions League</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Union Berlin</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Arsenal</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>1-1</t>
+          <t>2-3</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H43" t="n">
-        <v>659</v>
+        <v>37.98</v>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>Empatado</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
@@ -2562,40 +2564,40 @@
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
-        <v>45286</v>
+        <v>45277</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Burnley</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Villarreal</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>0-2</t>
+          <t>4-1</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H44" t="n">
-        <v>659</v>
+        <v>39.3</v>
       </c>
       <c r="I44" t="inlineStr">
         <is>
@@ -2604,47 +2606,47 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
-        <v>45292</v>
+        <v>45281</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Deportivo Alavés</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Newcastle</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>4-2</t>
+          <t>0-1</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H45" t="n">
-        <v>658.8</v>
+        <v>39.77</v>
       </c>
       <c r="I45" t="inlineStr">
         <is>
@@ -2653,47 +2655,47 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
-        <v>45298</v>
+        <v>45294</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>FA Cup</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Arsenal</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Mallorca</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>0-2</t>
+          <t>1-0</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
       <c r="H46" t="n">
-        <v>650</v>
+        <v>39.41</v>
       </c>
       <c r="I46" t="inlineStr">
         <is>
@@ -2702,47 +2704,47 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
-        <v>45301</v>
+        <v>45297</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>EFL Cup</t>
+          <t>Copa del Rey</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Arandina</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Fulham</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>2-1</t>
+          <t>1-3</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H47" t="n">
-        <v>626.4</v>
+        <v>39.98</v>
       </c>
       <c r="I47" t="inlineStr">
         <is>
@@ -2751,47 +2753,47 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
-        <v>45312</v>
+        <v>45301</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Supercopa de España</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>AFC Bournemouth</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Atlético</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>0-4</t>
+          <t>5-3</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>5</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H48" t="n">
-        <v>580.6</v>
+        <v>38.977</v>
       </c>
       <c r="I48" t="inlineStr">
         <is>
@@ -2800,38 +2802,38 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
-        <v>45315</v>
+        <v>45305</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>EFL Cup</t>
+          <t>Supercopa de España</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Fulham</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Barcelona</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>1-1</t>
+          <t>4-1</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
@@ -2840,11 +2842,11 @@
         </is>
       </c>
       <c r="H49" t="n">
-        <v>609.4</v>
+        <v>39.797</v>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>Empatado</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
@@ -2856,31 +2858,31 @@
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
-        <v>45319</v>
+        <v>45309</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>FA Cup</t>
+          <t>Copa del Rey</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Atlético</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Norwich City</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>5-2</t>
+          <t>4-2</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
@@ -2889,56 +2891,58 @@
         </is>
       </c>
       <c r="H50" t="n">
-        <v>602.4</v>
+        <v>39.214</v>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Perdido</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="K50" t="inlineStr"/>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="K50" t="n">
+        <v>153.5735694237965</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
-        <v>45322</v>
+        <v>45312</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Chelsea</t>
+          <t>Almería</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>4-1</t>
+          <t>3-2</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H51" t="n">
-        <v>598.8</v>
+        <v>39.75</v>
       </c>
       <c r="I51" t="inlineStr">
         <is>
@@ -2954,91 +2958,89 @@
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
-        <v>45326</v>
+        <v>45318</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Arsenal</t>
+          <t>Las Palmas</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>3-1</t>
+          <t>1-2</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H52" t="n">
-        <v>594</v>
+        <v>35.66</v>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="K52" t="n">
-        <v>-43.62014859710121</v>
-      </c>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
-        <v>45332</v>
+        <v>45323</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Getafe</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Burnley</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>3-1</t>
+          <t>0-2</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H53" t="n">
-        <v>581.6</v>
+        <v>36.61</v>
       </c>
       <c r="I53" t="inlineStr">
         <is>
@@ -3054,26 +3056,26 @@
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
-        <v>45339</v>
+        <v>45326</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Brentford</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Atlético</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>1-4</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -3083,46 +3085,46 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H54" t="n">
-        <v>599.6</v>
+        <v>36.46</v>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Empatado</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
-        <v>45343</v>
+        <v>45332</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Luton Town</t>
+          <t>Girona</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>4-1</t>
+          <t>4-0</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -3132,11 +3134,11 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H55" t="n">
-        <v>601</v>
+        <v>36.21</v>
       </c>
       <c r="I55" t="inlineStr">
         <is>
@@ -3152,21 +3154,21 @@
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
-        <v>45347</v>
+        <v>45335</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>EFL Cup</t>
+          <t>Champions League</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Chelsea</t>
+          <t>RB Leipzig</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -3185,7 +3187,7 @@
         </is>
       </c>
       <c r="H56" t="n">
-        <v>636.4</v>
+        <v>36.39</v>
       </c>
       <c r="I56" t="inlineStr">
         <is>
@@ -3201,89 +3203,89 @@
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
-        <v>45350</v>
+        <v>45340</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>FA Cup</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Rayo Vallecano</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Southampton</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>3-0</t>
+          <t>1-1</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="H57" t="n">
-        <v>649.2</v>
+        <v>36.45</v>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Empatado</t>
         </is>
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" s="2" t="n">
-        <v>45353</v>
+        <v>45347</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Nottingham Forest</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Sevilla</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>0-1</t>
+          <t>1-0</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="H58" t="n">
-        <v>682.4</v>
+        <v>36.94</v>
       </c>
       <c r="I58" t="inlineStr">
         <is>
@@ -3299,70 +3301,70 @@
     </row>
     <row r="59">
       <c r="A59" s="2" t="n">
-        <v>45358</v>
+        <v>45353</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Europa League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Sparta Praha</t>
+          <t>Valencia</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>1-5</t>
+          <t>2-2</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H59" t="n">
-        <v>664.4</v>
+        <v>37.74</v>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Empatado</t>
         </is>
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" s="2" t="n">
-        <v>45361</v>
+        <v>45357</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Champions League</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Manchester City</t>
+          <t>RB Leipzig</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -3381,7 +3383,7 @@
         </is>
       </c>
       <c r="H60" t="n">
-        <v>660</v>
+        <v>38.5</v>
       </c>
       <c r="I60" t="inlineStr">
         <is>
@@ -3397,40 +3399,40 @@
     </row>
     <row r="61">
       <c r="A61" s="2" t="n">
-        <v>45365</v>
+        <v>45361</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Europa League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Sparta Praha</t>
+          <t>Celta</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>6-1</t>
+          <t>4-0</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H61" t="n">
-        <v>646</v>
+        <v>38.77</v>
       </c>
       <c r="I61" t="inlineStr">
         <is>
@@ -3446,54 +3448,52 @@
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
-        <v>45368</v>
+        <v>45367</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>FA Cup</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Manchester United</t>
+          <t>Osasuna</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>4-3</t>
+          <t>2-4</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
           <t>4</t>
         </is>
       </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
       <c r="H62" t="n">
-        <v>650.2</v>
+        <v>40.14</v>
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>Perdido</t>
+          <t>Ganado</t>
         </is>
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="K62" t="n">
-        <v>24.53709477421653</v>
-      </c>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" s="2" t="n">
@@ -3501,22 +3501,22 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Primera División</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Brighton &amp; Hove Albion</t>
+          <t>Athletic</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>2-1</t>
+          <t>2-0</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -3526,11 +3526,11 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="H63" t="n">
-        <v>678.6</v>
+        <v>38.48</v>
       </c>
       <c r="I63" t="inlineStr">
         <is>
@@ -3546,26 +3546,26 @@
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
-        <v>45386</v>
+        <v>45391</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Premier League</t>
+          <t>Champions League</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Liverpool</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Sheffield United</t>
+          <t>Manchester City</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>3-1</t>
+          <t>3-3</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -3575,123 +3575,23 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="H64" t="n">
-        <v>702</v>
+        <v>37.78</v>
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>Ganado</t>
+          <t>Empatado</t>
         </is>
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>NO SE REALIZA OPERACION</t>
         </is>
       </c>
       <c r="K64" t="inlineStr"/>
-    </row>
-    <row r="65">
-      <c r="A65" s="2" t="n">
-        <v>45389</v>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>Premier League</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>Manchester United</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>Liverpool</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>2-2</t>
-        </is>
-      </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="H65" t="n">
-        <v>699</v>
-      </c>
-      <c r="I65" t="inlineStr">
-        <is>
-          <t>Empatado</t>
-        </is>
-      </c>
-      <c r="J65" t="inlineStr">
-        <is>
-          <t>NO SE REALIZA OPERACION</t>
-        </is>
-      </c>
-      <c r="K65" t="inlineStr"/>
-    </row>
-    <row r="66">
-      <c r="A66" s="2" t="n">
-        <v>45393</v>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>Europa League</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>Liverpool</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>Atalanta</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>0-3</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="H66" t="n">
-        <v>666</v>
-      </c>
-      <c r="I66" t="inlineStr">
-        <is>
-          <t>Perdido</t>
-        </is>
-      </c>
-      <c r="J66" t="inlineStr">
-        <is>
-          <t>-1</t>
-        </is>
-      </c>
-      <c r="K66" t="n">
-        <v>-6.984969053934574</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>